<commit_message>
add log for colombo module
</commit_message>
<xml_diff>
--- a/hammer-project/hammer-shark/civicdata_query/1_result.xlsx
+++ b/hammer-project/hammer-shark/civicdata_query/1_result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Test 1</t>
   </si>
@@ -108,13 +108,49 @@
   </si>
   <si>
     <t>0.3 0.3 0.90 3 10</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>0.2 0.2 0.90 3 100</t>
+  </si>
+  <si>
+    <t>0.3 0.3 0.90 3 100</t>
+  </si>
+  <si>
+    <t>Test 7</t>
+  </si>
+  <si>
+    <t>Test 8</t>
+  </si>
+  <si>
+    <t>0.2 0.2 0.90 3 1000</t>
+  </si>
+  <si>
+    <t>0.3 0.3 0.90 3 1000</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +178,11 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="3">
@@ -197,11 +238,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -491,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -507,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -535,7 +578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -543,23 +586,23 @@
         <v>26</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1">
         <v>17</v>
       </c>
       <c r="G3" s="1">
-        <v>9</v>
+        <v>567</v>
       </c>
       <c r="H3" s="1">
         <f>SUM(B3:G3)</f>
-        <v>199</v>
+        <v>721</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
@@ -568,7 +611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -588,11 +631,11 @@
         <v>14</v>
       </c>
       <c r="G4" s="1">
-        <v>9</v>
+        <v>567</v>
       </c>
       <c r="H4" s="1">
         <f>SUM(B4:G4)</f>
-        <v>188</v>
+        <v>746</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
@@ -601,7 +644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -621,11 +664,11 @@
         <v>12</v>
       </c>
       <c r="G5" s="1">
-        <v>9</v>
+        <v>567</v>
       </c>
       <c r="H5" s="1">
         <f>SUM(B5:G5)</f>
-        <v>161</v>
+        <v>719</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>17</v>
@@ -634,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -654,11 +697,11 @@
         <v>7</v>
       </c>
       <c r="G6" s="1">
-        <v>10</v>
+        <v>568</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(B6:G6)</f>
-        <v>145</v>
+        <v>703</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -667,7 +710,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1044</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SUM(B7:G7)</f>
+        <v>1100</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>21</v>
       </c>
@@ -675,120 +743,254 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <f>SUM(B8:G8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <f>SUM(B9:G9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <f>SUM(B10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D21" s="1">
         <v>3</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E21" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F21" s="1">
         <v>5</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G21" s="1">
         <v>6</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1">
-        <f>SUM(B11:G11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B22" s="1">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1">
-        <f>SUM(B12:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1">
+        <v>435</v>
+      </c>
+      <c r="H22" s="1">
+        <f>SUM(B22:G22)</f>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1">
+        <v>249</v>
+      </c>
+      <c r="H23" s="1">
+        <f>SUM(B23:G23)</f>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1">
-        <f>SUM(B13:G13)</f>
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="B24" s="1">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7</v>
+      </c>
+      <c r="H24" s="1">
+        <f>SUM(B24:G24)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1">
-        <f>SUM(B14:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J15" t="s">
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
         <v>3</v>
       </c>
-      <c r="K15" t="s">
-        <v>26</v>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1">
+        <f>SUM(B25:G25)</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>